<commit_message>
Fixed error in MILP version switch
</commit_message>
<xml_diff>
--- a/Code/Results/Results_Summary.xlsx
+++ b/Code/Results/Results_Summary.xlsx
@@ -411,7 +411,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,6 +432,26 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Step 1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Step 2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Step 3</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Step 4</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
@@ -448,7 +468,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>131.13</v>
+        <v>54.67</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>54.67</v>
       </c>
     </row>
     <row r="3">
@@ -463,7 +495,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>529.75</v>
+        <v>227.2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>227.2</v>
       </c>
     </row>
     <row r="4">
@@ -478,7 +522,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>32.32</v>
+        <v>2.83</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2.83</v>
       </c>
     </row>
   </sheetData>
@@ -492,7 +548,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,6 +579,26 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Step 1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Step 2</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Step 3</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Step 4</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
@@ -548,8 +624,28 @@
           <t>kUSD</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>376.18</v>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>198.678</v>
       </c>
     </row>
     <row r="3">
@@ -571,8 +667,28 @@
           <t>kUSD</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>376.18</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>198.678</v>
       </c>
     </row>
     <row r="4">
@@ -596,8 +712,28 @@
           <t>kUSD</t>
         </is>
       </c>
-      <c r="E4" t="n">
-        <v>147.969</v>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>123.82</v>
       </c>
     </row>
     <row r="5">
@@ -621,8 +757,28 @@
           <t>kUSD</t>
         </is>
       </c>
-      <c r="E5" t="n">
-        <v>47.479</v>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>50.609</v>
       </c>
     </row>
     <row r="6">
@@ -644,8 +800,28 @@
           <t>kUSD</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>184.297</v>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>24.249</v>
       </c>
     </row>
     <row r="7">
@@ -669,8 +845,28 @@
           <t>kUSD</t>
         </is>
       </c>
-      <c r="E7" t="n">
-        <v>-3.565</v>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>-0</v>
       </c>
     </row>
     <row r="8">
@@ -694,8 +890,28 @@
           <t>USD/kWh</t>
         </is>
       </c>
-      <c r="E8" t="n">
-        <v>0.205</v>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>0.2812</v>
       </c>
     </row>
     <row r="9">
@@ -717,8 +933,28 @@
           <t>USD/kWh</t>
         </is>
       </c>
-      <c r="E9" t="n">
-        <v>0.205</v>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>0.2812</v>
       </c>
     </row>
     <row r="10">
@@ -743,7 +979,19 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>107.199</v>
+        <v>58.766</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>58.766</v>
       </c>
     </row>
     <row r="11">
@@ -764,7 +1012,19 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>27.841</v>
+        <v>49.301</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>49.301</v>
       </c>
     </row>
     <row r="12">
@@ -785,81 +1045,137 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>12.928</v>
+        <v>-23.587</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-23.587</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
+          <t>National Grid</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>kUSD</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>31.053</v>
+      </c>
+      <c r="G13" t="n">
+        <v>19.281</v>
+      </c>
+      <c r="H13" t="n">
+        <v>11.972</v>
+      </c>
+      <c r="I13" t="n">
+        <v>62.307</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n"/>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
           <t>National grid</t>
         </is>
       </c>
-      <c r="C13" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D13" s="1" t="inlineStr">
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D14" s="1" t="inlineStr">
         <is>
           <t>kUSD</t>
         </is>
       </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
         <is>
           <t>Fixed cost</t>
         </is>
       </c>
-      <c r="B14" s="1" t="inlineStr">
+      <c r="B15" s="1" t="inlineStr">
         <is>
           <t>PV panels</t>
         </is>
       </c>
-      <c r="C14" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D14" s="1" t="inlineStr">
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D15" s="1" t="inlineStr">
         <is>
           <t>kUSD</t>
         </is>
       </c>
-      <c r="E14" t="n">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n"/>
-      <c r="B15" s="1" t="inlineStr">
-        <is>
-          <t>Battery bank</t>
-        </is>
-      </c>
-      <c r="C15" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D15" s="1" t="inlineStr">
-        <is>
-          <t>kUSD</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>18.697</v>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>11.171</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>Diesel Genset</t>
+          <t>Battery bank</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr">
@@ -872,63 +1188,121 @@
           <t>kUSD</t>
         </is>
       </c>
-      <c r="E16" t="n">
-        <v>6.482</v>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>38.686</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="inlineStr">
         <is>
+          <t>Diesel Genset</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D17" s="1" t="inlineStr">
+        <is>
+          <t>kUSD</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>0.752</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n"/>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
           <t>National Grid</t>
         </is>
       </c>
-      <c r="C17" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D17" s="1" t="inlineStr">
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D18" s="1" t="inlineStr">
         <is>
           <t>kUSD</t>
         </is>
       </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>Lost load cost</t>
-        </is>
-      </c>
-      <c r="B18" s="1" t="inlineStr">
-        <is>
-          <t>System</t>
-        </is>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1" t="inlineStr">
-        <is>
-          <t>kUSD</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Replacement cost</t>
+          <t>Lost load cost</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>Battery bank</t>
+          <t>System</t>
         </is>
       </c>
       <c r="C19" s="1" t="n">
@@ -939,19 +1313,39 @@
           <t>kUSD</t>
         </is>
       </c>
-      <c r="E19" t="n">
-        <v>27.883</v>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Fuel cost</t>
+          <t>Replacement cost</t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>Diesel</t>
+          <t>Battery bank</t>
         </is>
       </c>
       <c r="C20" s="1" t="n">
@@ -962,19 +1356,39 @@
           <t>kUSD</t>
         </is>
       </c>
-      <c r="E20" t="n">
-        <v>156.414</v>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>11.012</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Grid electricity cost</t>
+          <t>Fuel cost</t>
         </is>
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>National Grid</t>
+          <t>Diesel</t>
         </is>
       </c>
       <c r="C21" s="1" t="n">
@@ -985,14 +1399,34 @@
           <t>kUSD</t>
         </is>
       </c>
-      <c r="E21" t="n">
-        <v>0</v>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>13.237</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Grid electricity revenue</t>
+          <t>Grid electricity cost</t>
         </is>
       </c>
       <c r="B22" s="1" t="inlineStr">
@@ -1008,19 +1442,39 @@
           <t>kUSD</t>
         </is>
       </c>
-      <c r="E22" t="n">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Fuel CO2 emission</t>
+          <t>Grid electricity revenue</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>System</t>
+          <t>National Grid</t>
         </is>
       </c>
       <c r="C23" s="1" t="n">
@@ -1028,17 +1482,37 @@
       </c>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>ton</t>
-        </is>
-      </c>
-      <c r="E23" t="n">
-        <v>1060.636</v>
+          <t>kUSD</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Grid CO2 emission</t>
+          <t>Fuel CO2 emission</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr">
@@ -1054,44 +1528,82 @@
           <t>ton</t>
         </is>
       </c>
-      <c r="E24" t="n">
-        <v>0</v>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>39.18</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>RES CO2 emission</t>
+          <t>Grid CO2 emission</t>
         </is>
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>RES</t>
-        </is>
-      </c>
-      <c r="C25" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="D25" s="1" t="inlineStr">
         <is>
           <t>ton</t>
         </is>
       </c>
-      <c r="E25" t="n">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>GEN CO2 emission</t>
+          <t>RES CO2 emission</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>GEN</t>
+          <t>RES</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr">
@@ -1104,19 +1616,39 @@
           <t>ton</t>
         </is>
       </c>
-      <c r="E26" t="n">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>BESS CO2 emission</t>
+          <t>GEN CO2 emission</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>BESS</t>
+          <t>GEN</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr">
@@ -1129,37 +1661,122 @@
           <t>ton</t>
         </is>
       </c>
-      <c r="E27" t="n">
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
+          <t>BESS CO2 emission</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>BESS</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D28" s="1" t="inlineStr">
+        <is>
+          <t>ton</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
           <t>TOTAL CO2 emission</t>
         </is>
       </c>
-      <c r="B28" s="1" t="inlineStr">
+      <c r="B29" s="1" t="inlineStr">
         <is>
           <t>System</t>
         </is>
       </c>
-      <c r="C28" s="1" t="n">
+      <c r="C29" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D28" s="1" t="inlineStr">
+      <c r="D29" s="1" t="inlineStr">
         <is>
           <t>ton</t>
         </is>
       </c>
-      <c r="E28" t="n">
-        <v>1060.636</v>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>39.18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A18"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -1171,7 +1788,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1368,13 +1985,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C6" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -1383,10 +2000,10 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>3.07</v>
+        <v>1.29</v>
       </c>
       <c r="H6" t="n">
-        <v>0.52</v>
+        <v>1.55</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -1402,13 +2019,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C7" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -1417,10 +2034,10 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>3.41</v>
+        <v>1.29</v>
       </c>
       <c r="H7" t="n">
-        <v>1.39</v>
+        <v>1.55</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -1436,13 +2053,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C8" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -1451,10 +2068,10 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>3.49</v>
+        <v>1.29</v>
       </c>
       <c r="H8" t="n">
-        <v>1.78</v>
+        <v>1.55</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -1470,13 +2087,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C9" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -1485,10 +2102,10 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>3.69</v>
+        <v>1.29</v>
       </c>
       <c r="H9" t="n">
-        <v>4.22</v>
+        <v>1.55</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -1504,13 +2121,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C10" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -1519,10 +2136,10 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>3.66</v>
+        <v>1.29</v>
       </c>
       <c r="H10" t="n">
-        <v>13.87</v>
+        <v>1.55</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -1538,13 +2155,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C11" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -1553,10 +2170,10 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>3.64</v>
+        <v>1.29</v>
       </c>
       <c r="H11" t="n">
-        <v>15.21</v>
+        <v>1.55</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -1572,13 +2189,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C12" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -1587,10 +2204,10 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>3.59</v>
+        <v>1.29</v>
       </c>
       <c r="H12" t="n">
-        <v>28.04</v>
+        <v>1.55</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
@@ -1606,13 +2223,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C13" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -1621,10 +2238,10 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>3.59</v>
+        <v>1.29</v>
       </c>
       <c r="H13" t="n">
-        <v>28.26</v>
+        <v>1.55</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -1640,13 +2257,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C14" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -1655,10 +2272,10 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>3.58</v>
+        <v>1.29</v>
       </c>
       <c r="H14" t="n">
-        <v>29.76</v>
+        <v>1.55</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -1674,13 +2291,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C15" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -1689,10 +2306,10 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>3.58</v>
+        <v>1.29</v>
       </c>
       <c r="H15" t="n">
-        <v>30.35</v>
+        <v>1.55</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -1708,13 +2325,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C16" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1723,10 +2340,10 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>3.43</v>
+        <v>1.29</v>
       </c>
       <c r="H16" t="n">
-        <v>37.98</v>
+        <v>1.55</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -1742,13 +2359,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C17" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1757,10 +2374,10 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>3.43</v>
+        <v>1.29</v>
       </c>
       <c r="H17" t="n">
-        <v>38.14</v>
+        <v>1.55</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1776,13 +2393,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C18" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -1791,10 +2408,10 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>3.44</v>
+        <v>1.29</v>
       </c>
       <c r="H18" t="n">
-        <v>41.93</v>
+        <v>1.55</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -1810,13 +2427,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C19" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -1825,10 +2442,10 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>3.39</v>
+        <v>1.29</v>
       </c>
       <c r="H19" t="n">
-        <v>45.83</v>
+        <v>1.55</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
@@ -1844,13 +2461,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C20" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -1859,10 +2476,10 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>3.37</v>
+        <v>1.29</v>
       </c>
       <c r="H20" t="n">
-        <v>48.58</v>
+        <v>1.55</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
@@ -1878,13 +2495,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C21" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -1893,10 +2510,10 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>3.37</v>
+        <v>1.29</v>
       </c>
       <c r="H21" t="n">
-        <v>48.57</v>
+        <v>1.55</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
@@ -1912,13 +2529,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2.78</v>
+        <v>1.31</v>
       </c>
       <c r="C22" t="n">
-        <v>2.33</v>
+        <v>4.54</v>
       </c>
       <c r="D22" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -1927,15 +2544,117 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>3.36</v>
+        <v>1.29</v>
       </c>
       <c r="H22" t="n">
-        <v>48.56</v>
+        <v>1.55</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
       </c>
       <c r="J22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Year 18</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="C23" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Year 19</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="C24" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>Year 20</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="C25" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1953,7 +2672,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2028,16 +2747,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.95</v>
+        <v>2.06</v>
       </c>
       <c r="C4" t="n">
-        <v>99.47</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>39.93</v>
+        <v>16.22</v>
       </c>
       <c r="E4" t="n">
-        <v>53.83</v>
+        <v>52.05</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -2050,16 +2769,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.26</v>
+        <v>2.06</v>
       </c>
       <c r="C5" t="n">
-        <v>98.59</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>32.47</v>
+        <v>16.12</v>
       </c>
       <c r="E5" t="n">
-        <v>52.77</v>
+        <v>52.05</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -2072,16 +2791,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.83</v>
+        <v>2.06</v>
       </c>
       <c r="C6" t="n">
-        <v>98.2</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D6" t="n">
-        <v>31.1</v>
+        <v>16.12</v>
       </c>
       <c r="E6" t="n">
-        <v>52.58</v>
+        <v>52.05</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -2094,16 +2813,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5.98</v>
+        <v>2.06</v>
       </c>
       <c r="C7" t="n">
-        <v>95.84999999999999</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D7" t="n">
-        <v>25.03</v>
+        <v>16.12</v>
       </c>
       <c r="E7" t="n">
-        <v>49.78</v>
+        <v>52.05</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -2116,16 +2835,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>15.5</v>
+        <v>2.06</v>
       </c>
       <c r="C8" t="n">
-        <v>87.54000000000001</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D8" t="n">
-        <v>14.54</v>
+        <v>16.12</v>
       </c>
       <c r="E8" t="n">
-        <v>38.81</v>
+        <v>52.05</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -2138,16 +2857,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>16.46</v>
+        <v>2.06</v>
       </c>
       <c r="C9" t="n">
-        <v>86.5</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D9" t="n">
-        <v>12.98</v>
+        <v>16.12</v>
       </c>
       <c r="E9" t="n">
-        <v>37.43</v>
+        <v>52.05</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -2160,16 +2879,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>25.39</v>
+        <v>2.06</v>
       </c>
       <c r="C10" t="n">
-        <v>77.66</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>7.57</v>
+        <v>16.12</v>
       </c>
       <c r="E10" t="n">
-        <v>30.89</v>
+        <v>52.05</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -2182,16 +2901,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>25.51</v>
+        <v>2.06</v>
       </c>
       <c r="C11" t="n">
-        <v>77.52</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D11" t="n">
-        <v>7.44</v>
+        <v>16.12</v>
       </c>
       <c r="E11" t="n">
-        <v>30.78</v>
+        <v>52.05</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -2204,16 +2923,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>26.29</v>
+        <v>2.06</v>
       </c>
       <c r="C12" t="n">
-        <v>76.61</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D12" t="n">
-        <v>6.66</v>
+        <v>16.12</v>
       </c>
       <c r="E12" t="n">
-        <v>30.02</v>
+        <v>52.05</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -2226,16 +2945,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>26.66</v>
+        <v>2.06</v>
       </c>
       <c r="C13" t="n">
-        <v>76.25</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D13" t="n">
-        <v>6.59</v>
+        <v>16.12</v>
       </c>
       <c r="E13" t="n">
-        <v>29.85</v>
+        <v>52.05</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -2248,16 +2967,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>29.89</v>
+        <v>2.06</v>
       </c>
       <c r="C14" t="n">
-        <v>71.95999999999999</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D14" t="n">
-        <v>2.25</v>
+        <v>16.12</v>
       </c>
       <c r="E14" t="n">
-        <v>25.68</v>
+        <v>52.05</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -2270,16 +2989,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>29.99</v>
+        <v>2.06</v>
       </c>
       <c r="C15" t="n">
-        <v>71.87</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D15" t="n">
-        <v>2.27</v>
+        <v>16.12</v>
       </c>
       <c r="E15" t="n">
-        <v>25.64</v>
+        <v>52.05</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -2292,16 +3011,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>31.79</v>
+        <v>2.06</v>
       </c>
       <c r="C16" t="n">
-        <v>69.92</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D16" t="n">
-        <v>1.54</v>
+        <v>16.12</v>
       </c>
       <c r="E16" t="n">
-        <v>24.81</v>
+        <v>52.05</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -2314,16 +3033,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>33.56</v>
+        <v>2.06</v>
       </c>
       <c r="C17" t="n">
-        <v>68.01000000000001</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D17" t="n">
-        <v>1.02</v>
+        <v>16.12</v>
       </c>
       <c r="E17" t="n">
-        <v>23.6</v>
+        <v>52.05</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -2336,16 +3055,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>34.76</v>
+        <v>2.06</v>
       </c>
       <c r="C18" t="n">
-        <v>66.73</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D18" t="n">
-        <v>0.71</v>
+        <v>16.12</v>
       </c>
       <c r="E18" t="n">
-        <v>22.88</v>
+        <v>52.05</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -2358,16 +3077,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>34.76</v>
+        <v>2.06</v>
       </c>
       <c r="C19" t="n">
-        <v>66.73999999999999</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D19" t="n">
-        <v>0.74</v>
+        <v>16.12</v>
       </c>
       <c r="E19" t="n">
-        <v>22.88</v>
+        <v>52.05</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -2380,18 +3099,84 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>34.75</v>
+        <v>2.06</v>
       </c>
       <c r="C20" t="n">
-        <v>66.73999999999999</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D20" t="n">
-        <v>0.73</v>
+        <v>16.12</v>
       </c>
       <c r="E20" t="n">
-        <v>22.85</v>
+        <v>52.05</v>
       </c>
       <c r="F20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>Year 18</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="C21" t="n">
+        <v>98.40000000000001</v>
+      </c>
+      <c r="D21" t="n">
+        <v>16.12</v>
+      </c>
+      <c r="E21" t="n">
+        <v>52.05</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Year 19</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="C22" t="n">
+        <v>98.40000000000001</v>
+      </c>
+      <c r="D22" t="n">
+        <v>16.12</v>
+      </c>
+      <c r="E22" t="n">
+        <v>52.05</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Year 20</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="C23" t="n">
+        <v>98.40000000000001</v>
+      </c>
+      <c r="D23" t="n">
+        <v>16.15</v>
+      </c>
+      <c r="E23" t="n">
+        <v>52.05</v>
+      </c>
+      <c r="F23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2406,7 +3191,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2535,16 +3320,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.95</v>
+        <v>2.06</v>
       </c>
       <c r="C6" t="n">
-        <v>99.47</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D6" t="n">
-        <v>39.93</v>
+        <v>16.22</v>
       </c>
       <c r="E6" t="n">
-        <v>53.83</v>
+        <v>52.05</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -2557,16 +3342,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.26</v>
+        <v>2.06</v>
       </c>
       <c r="C7" t="n">
-        <v>98.59</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D7" t="n">
-        <v>32.47</v>
+        <v>16.12</v>
       </c>
       <c r="E7" t="n">
-        <v>52.77</v>
+        <v>52.05</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -2579,16 +3364,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.83</v>
+        <v>2.06</v>
       </c>
       <c r="C8" t="n">
-        <v>98.2</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D8" t="n">
-        <v>31.1</v>
+        <v>16.12</v>
       </c>
       <c r="E8" t="n">
-        <v>52.58</v>
+        <v>52.05</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -2601,16 +3386,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5.98</v>
+        <v>2.06</v>
       </c>
       <c r="C9" t="n">
-        <v>95.84999999999999</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D9" t="n">
-        <v>25.03</v>
+        <v>16.12</v>
       </c>
       <c r="E9" t="n">
-        <v>49.78</v>
+        <v>52.05</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -2623,16 +3408,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>15.5</v>
+        <v>2.06</v>
       </c>
       <c r="C10" t="n">
-        <v>87.54000000000001</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>14.54</v>
+        <v>16.12</v>
       </c>
       <c r="E10" t="n">
-        <v>38.81</v>
+        <v>52.05</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -2645,16 +3430,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>16.46</v>
+        <v>2.06</v>
       </c>
       <c r="C11" t="n">
-        <v>86.5</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D11" t="n">
-        <v>12.98</v>
+        <v>16.12</v>
       </c>
       <c r="E11" t="n">
-        <v>37.43</v>
+        <v>52.05</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -2667,16 +3452,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>25.39</v>
+        <v>2.06</v>
       </c>
       <c r="C12" t="n">
-        <v>77.66</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D12" t="n">
-        <v>7.57</v>
+        <v>16.12</v>
       </c>
       <c r="E12" t="n">
-        <v>30.89</v>
+        <v>52.05</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -2689,16 +3474,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>25.51</v>
+        <v>2.06</v>
       </c>
       <c r="C13" t="n">
-        <v>77.52</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D13" t="n">
-        <v>7.44</v>
+        <v>16.12</v>
       </c>
       <c r="E13" t="n">
-        <v>30.78</v>
+        <v>52.05</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -2711,16 +3496,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>26.29</v>
+        <v>2.06</v>
       </c>
       <c r="C14" t="n">
-        <v>76.61</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D14" t="n">
-        <v>6.66</v>
+        <v>16.12</v>
       </c>
       <c r="E14" t="n">
-        <v>30.02</v>
+        <v>52.05</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -2733,16 +3518,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>26.66</v>
+        <v>2.06</v>
       </c>
       <c r="C15" t="n">
-        <v>76.25</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D15" t="n">
-        <v>6.59</v>
+        <v>16.12</v>
       </c>
       <c r="E15" t="n">
-        <v>29.85</v>
+        <v>52.05</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -2755,16 +3540,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>29.89</v>
+        <v>2.06</v>
       </c>
       <c r="C16" t="n">
-        <v>71.95999999999999</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D16" t="n">
-        <v>2.25</v>
+        <v>16.12</v>
       </c>
       <c r="E16" t="n">
-        <v>25.68</v>
+        <v>52.05</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -2777,16 +3562,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>29.99</v>
+        <v>2.06</v>
       </c>
       <c r="C17" t="n">
-        <v>71.87</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D17" t="n">
-        <v>2.27</v>
+        <v>16.12</v>
       </c>
       <c r="E17" t="n">
-        <v>25.64</v>
+        <v>52.05</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -2799,16 +3584,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>31.79</v>
+        <v>2.06</v>
       </c>
       <c r="C18" t="n">
-        <v>69.92</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D18" t="n">
-        <v>1.54</v>
+        <v>16.12</v>
       </c>
       <c r="E18" t="n">
-        <v>24.81</v>
+        <v>52.05</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -2821,16 +3606,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>33.56</v>
+        <v>2.06</v>
       </c>
       <c r="C19" t="n">
-        <v>68.01000000000001</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D19" t="n">
-        <v>1.02</v>
+        <v>16.12</v>
       </c>
       <c r="E19" t="n">
-        <v>23.6</v>
+        <v>52.05</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -2843,16 +3628,16 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>34.76</v>
+        <v>2.06</v>
       </c>
       <c r="C20" t="n">
-        <v>66.73</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D20" t="n">
-        <v>0.71</v>
+        <v>16.12</v>
       </c>
       <c r="E20" t="n">
-        <v>22.88</v>
+        <v>52.05</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -2865,16 +3650,16 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>34.76</v>
+        <v>2.06</v>
       </c>
       <c r="C21" t="n">
-        <v>66.73999999999999</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D21" t="n">
-        <v>0.74</v>
+        <v>16.12</v>
       </c>
       <c r="E21" t="n">
-        <v>22.88</v>
+        <v>52.05</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -2887,18 +3672,84 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>34.75</v>
+        <v>2.06</v>
       </c>
       <c r="C22" t="n">
-        <v>66.73999999999999</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="D22" t="n">
-        <v>0.73</v>
+        <v>16.12</v>
       </c>
       <c r="E22" t="n">
-        <v>22.85</v>
+        <v>52.05</v>
       </c>
       <c r="F22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Year 18</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="C23" t="n">
+        <v>98.40000000000001</v>
+      </c>
+      <c r="D23" t="n">
+        <v>16.12</v>
+      </c>
+      <c r="E23" t="n">
+        <v>52.05</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Year 19</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="C24" t="n">
+        <v>98.40000000000001</v>
+      </c>
+      <c r="D24" t="n">
+        <v>16.12</v>
+      </c>
+      <c r="E24" t="n">
+        <v>52.05</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>Year 20</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="C25" t="n">
+        <v>98.40000000000001</v>
+      </c>
+      <c r="D25" t="n">
+        <v>16.15</v>
+      </c>
+      <c r="E25" t="n">
+        <v>52.05</v>
+      </c>
+      <c r="F25" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>